<commit_message>
analyse amazon mturk result
</commit_message>
<xml_diff>
--- a/adversarialVPR/human-study/human-study-pre-test/experiment3-identify-speaker/info.xlsx
+++ b/adversarialVPR/human-study/human-study-pre-test/experiment3-identify-speaker/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\GolferChen.github.io\adversarialVPR\human-study\human-study-pre-test\experiment3-identify-speaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B67B5B-DAF4-4AA2-8789-09CF991BD982}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304688FE-7064-4178-886B-F66979C4D878}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="spk1" sheetId="1" r:id="rId1"/>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1020,7 +1020,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:H11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1307,8 +1307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>